<commit_message>
update logs & results
</commit_message>
<xml_diff>
--- a/metrics/metrics.xlsx
+++ b/metrics/metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="31">
   <si>
     <t>L0 RAW</t>
   </si>
@@ -115,6 +115,14 @@
   <si>
     <t>L1
 CONTRAST-ENHANCED DTW</t>
+  </si>
+  <si>
+    <t>L1 SIFT 
+RELOADED</t>
+  </si>
+  <si>
+    <t>L0 RAW
+RELOADED</t>
   </si>
 </sst>
 </file>
@@ -283,32 +291,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,6 +311,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,8 +650,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="4" t="s">
         <v>13</v>
       </c>
@@ -679,1221 +687,1568 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.96662599999999999</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.95763799999999999</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.92513800000000002</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.82979099999999995</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.95615799999999995</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0.957233</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0.88627599999999995</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.93703000000000003</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.97994999999999999</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.92435199999999995</v>
+      </c>
+      <c r="M2" s="8">
+        <f t="shared" ref="M2:M5" si="0">AVERAGE(C2:L2)</f>
+        <v>0.93201920000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.99463400000000002</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.99197199999999996</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.97673500000000002</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.88756199999999996</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0.97686600000000001</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.98284800000000005</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.93448200000000003</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0.96614999999999995</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0.99272199999999999</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.96907299999999996</v>
+      </c>
+      <c r="M3" s="10">
+        <f t="shared" si="0"/>
+        <v>0.96730439999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.96384499999999995</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.95303000000000004</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.93096599999999996</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.96977800000000003</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.96979000000000004</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.96925799999999995</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.97020899999999999</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.98013799999999995</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.98663599999999996</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.95810499999999998</v>
+      </c>
+      <c r="M4" s="10">
+        <f t="shared" si="0"/>
+        <v>0.96517549999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11">
+        <f t="shared" ref="C5:L5" si="1">AVERAGE(C2:C4)</f>
+        <v>0.97503499999999999</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.96754666666666667</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.94427966666666663</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.89571033333333328</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.96760466666666678</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.96977966666666671</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.93032233333333336</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.96110600000000002</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.98643599999999998</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.95050999999999997</v>
+      </c>
+      <c r="M5" s="12">
+        <f t="shared" si="0"/>
+        <v>0.95483303333333325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C8" s="7">
         <v>0.95937700000000004</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D8" s="7">
         <v>0.94340500000000005</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E8" s="7">
         <v>0.91778000000000004</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F8" s="7">
         <v>0.744981</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G8" s="7">
         <v>0.88614599999999999</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H8" s="7">
         <v>0.93544300000000002</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I8" s="7">
         <v>0.84814500000000004</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J8" s="7">
         <v>0.90102800000000005</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K8" s="7">
         <v>0.95463699999999996</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L8" s="7">
         <v>0.914794</v>
       </c>
-      <c r="M2" s="11">
-        <f>AVERAGE(C2:L2)</f>
+      <c r="M8" s="8">
+        <f>AVERAGE(C8:L8)</f>
         <v>0.90057360000000009</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C9" s="9">
         <v>0.99012999999999995</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D9" s="9">
         <v>0.98212200000000005</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E9" s="9">
         <v>0.97227799999999998</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F9" s="9">
         <v>0.84058100000000002</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G9" s="9">
         <v>0.93245299999999998</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H9" s="9">
         <v>0.97145899999999996</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I9" s="9">
         <v>0.91376100000000005</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J9" s="9">
         <v>0.94772999999999996</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K9" s="9">
         <v>0.978742</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L9" s="9">
         <v>0.96367700000000001</v>
       </c>
-      <c r="M3" s="14">
-        <f t="shared" ref="M3:M5" si="0">AVERAGE(C3:L3)</f>
+      <c r="M9" s="10">
+        <f t="shared" ref="M9:M11" si="2">AVERAGE(C9:L9)</f>
         <v>0.94929330000000012</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C10" s="9">
         <v>0.95464599999999999</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D10" s="9">
         <v>0.93232899999999996</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E10" s="9">
         <v>0.92330000000000001</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F10" s="9">
         <v>0.91258899999999998</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G10" s="9">
         <v>0.89958099999999996</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H10" s="9">
         <v>0.95069300000000001</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I10" s="9">
         <v>0.93723400000000001</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J10" s="9">
         <v>0.95316800000000002</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K10" s="9">
         <v>0.96304000000000001</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L10" s="9">
         <v>0.94977800000000001</v>
       </c>
-      <c r="M4" s="14">
-        <f t="shared" si="0"/>
+      <c r="M10" s="10">
+        <f t="shared" si="2"/>
         <v>0.93763580000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16">
-        <f>AVERAGE(C2:C4)</f>
+      <c r="C11" s="11">
+        <f>AVERAGE(C8:C10)</f>
         <v>0.96805099999999999</v>
       </c>
-      <c r="D5" s="16">
-        <f t="shared" ref="D5:L5" si="1">AVERAGE(D2:D4)</f>
+      <c r="D11" s="11">
+        <f t="shared" ref="D11:L11" si="3">AVERAGE(D8:D10)</f>
         <v>0.95261866666666661</v>
       </c>
-      <c r="E5" s="16">
-        <f t="shared" si="1"/>
+      <c r="E11" s="11">
+        <f t="shared" si="3"/>
         <v>0.93778600000000001</v>
       </c>
-      <c r="F5" s="16">
-        <f t="shared" si="1"/>
+      <c r="F11" s="11">
+        <f t="shared" si="3"/>
         <v>0.83271700000000004</v>
       </c>
-      <c r="G5" s="16">
-        <f t="shared" si="1"/>
+      <c r="G11" s="11">
+        <f t="shared" si="3"/>
         <v>0.90605999999999998</v>
       </c>
-      <c r="H5" s="16">
-        <f t="shared" si="1"/>
+      <c r="H11" s="11">
+        <f t="shared" si="3"/>
         <v>0.95253166666666667</v>
       </c>
-      <c r="I5" s="16">
-        <f t="shared" si="1"/>
+      <c r="I11" s="11">
+        <f t="shared" si="3"/>
         <v>0.89971333333333348</v>
       </c>
-      <c r="J5" s="16">
-        <f t="shared" si="1"/>
+      <c r="J11" s="11">
+        <f t="shared" si="3"/>
         <v>0.93397533333333327</v>
       </c>
-      <c r="K5" s="16">
-        <f t="shared" si="1"/>
+      <c r="K11" s="11">
+        <f t="shared" si="3"/>
         <v>0.96547299999999991</v>
       </c>
-      <c r="L5" s="16">
-        <f t="shared" si="1"/>
+      <c r="L11" s="11">
+        <f t="shared" si="3"/>
         <v>0.94274966666666671</v>
       </c>
-      <c r="M5" s="17">
-        <f t="shared" si="0"/>
+      <c r="M11" s="12">
+        <f t="shared" si="2"/>
         <v>0.92916756666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C12" s="7">
         <v>0.96744799999999997</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D12" s="7">
         <v>0.87690000000000001</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E12" s="7">
         <v>0.949461</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F12" s="7">
         <v>0.86264700000000005</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G12" s="7">
         <v>0.87574700000000005</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H12" s="7">
         <v>0.91896999999999995</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I12" s="7">
         <v>0.87146500000000005</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J12" s="7">
         <v>0.82650999999999997</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K12" s="7">
         <v>0.92917300000000003</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L12" s="7">
         <v>0.93343699999999996</v>
       </c>
-      <c r="M6" s="11">
-        <f t="shared" ref="M6:M13" si="2">AVERAGE(C6:L6)</f>
+      <c r="M12" s="8">
+        <f t="shared" ref="M12:M19" si="4">AVERAGE(C12:L12)</f>
         <v>0.90117579999999986</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C13" s="9">
         <v>0.99407800000000002</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D13" s="9">
         <v>0.94807799999999998</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E13" s="9">
         <v>0.98490200000000006</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F13" s="9">
         <v>0.90702199999999999</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G13" s="9">
         <v>0.90535299999999996</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H13" s="9">
         <v>0.96250199999999997</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I13" s="9">
         <v>0.92833299999999996</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J13" s="9">
         <v>0.88914899999999997</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K13" s="9">
         <v>0.94355500000000003</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L13" s="9">
         <v>0.97350999999999999</v>
       </c>
-      <c r="M7" s="14">
-        <f t="shared" si="2"/>
+      <c r="M13" s="10">
+        <f t="shared" si="4"/>
         <v>0.94364819999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C14" s="9">
         <v>0.96823300000000001</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D14" s="9">
         <v>0.93430899999999995</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E14" s="9">
         <v>0.94696000000000002</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F14" s="9">
         <v>0.95313899999999996</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G14" s="9">
         <v>0.92677299999999996</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H14" s="9">
         <v>0.89097000000000004</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I14" s="9">
         <v>0.96239699999999995</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J14" s="9">
         <v>0.91905499999999996</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K14" s="9">
         <v>0.93804900000000002</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L14" s="9">
         <v>0.95843999999999996</v>
       </c>
-      <c r="M8" s="14">
-        <f t="shared" si="2"/>
+      <c r="M14" s="10">
+        <f t="shared" si="4"/>
         <v>0.93983249999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16" t="s">
+    <row r="15" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16">
-        <f>AVERAGE(C6:C8)</f>
+      <c r="C15" s="11">
+        <f>AVERAGE(C12:C14)</f>
         <v>0.97658633333333345</v>
       </c>
-      <c r="D9" s="16">
-        <f t="shared" ref="D9:L9" si="3">AVERAGE(D6:D8)</f>
+      <c r="D15" s="11">
+        <f t="shared" ref="D15:L15" si="5">AVERAGE(D12:D14)</f>
         <v>0.91976233333333335</v>
       </c>
-      <c r="E9" s="16">
-        <f t="shared" si="3"/>
+      <c r="E15" s="11">
+        <f t="shared" si="5"/>
         <v>0.96044099999999999</v>
       </c>
-      <c r="F9" s="16">
-        <f t="shared" si="3"/>
+      <c r="F15" s="11">
+        <f t="shared" si="5"/>
         <v>0.90760266666666656</v>
       </c>
-      <c r="G9" s="16">
-        <f t="shared" si="3"/>
+      <c r="G15" s="11">
+        <f t="shared" si="5"/>
         <v>0.90262433333333325</v>
       </c>
-      <c r="H9" s="16">
-        <f t="shared" si="3"/>
+      <c r="H15" s="11">
+        <f t="shared" si="5"/>
         <v>0.92414733333333332</v>
       </c>
-      <c r="I9" s="16">
-        <f t="shared" si="3"/>
+      <c r="I15" s="11">
+        <f t="shared" si="5"/>
         <v>0.92073166666666673</v>
       </c>
-      <c r="J9" s="16">
-        <f t="shared" si="3"/>
+      <c r="J15" s="11">
+        <f t="shared" si="5"/>
         <v>0.87823799999999996</v>
       </c>
-      <c r="K9" s="16">
-        <f t="shared" si="3"/>
+      <c r="K15" s="11">
+        <f t="shared" si="5"/>
         <v>0.93692566666666666</v>
       </c>
-      <c r="L9" s="16">
-        <f t="shared" si="3"/>
+      <c r="L15" s="11">
+        <f t="shared" si="5"/>
         <v>0.95512900000000001</v>
       </c>
-      <c r="M9" s="17">
-        <f t="shared" si="2"/>
+      <c r="M15" s="12">
+        <f t="shared" si="4"/>
         <v>0.92821883333333322</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C16" s="7">
         <v>0.97147499999999998</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D16" s="7">
         <v>0.96263100000000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E16" s="7">
         <v>0.942195</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F16" s="7">
         <v>0.92396100000000003</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G16" s="7">
         <v>0.927199</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H16" s="7">
         <v>0.94241900000000001</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I16" s="7">
         <v>0.814446</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J16" s="7">
         <v>0.95148699999999997</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K16" s="7">
         <v>0.98028599999999999</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L16" s="7">
         <v>0.93706500000000004</v>
       </c>
-      <c r="M10" s="11">
-        <f t="shared" si="2"/>
+      <c r="M16" s="8">
+        <f t="shared" si="4"/>
         <v>0.93531640000000016</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C17" s="9">
         <v>0.99563800000000002</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D17" s="9">
         <v>0.99254200000000004</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E17" s="9">
         <v>0.98355400000000004</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F17" s="9">
         <v>0.94940599999999997</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G17" s="9">
         <v>0.95184100000000005</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H17" s="9">
         <v>0.97691700000000004</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I17" s="9">
         <v>0.89043399999999995</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J17" s="9">
         <v>0.97370599999999996</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K17" s="9">
         <v>0.992869</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L17" s="9">
         <v>0.97504000000000002</v>
       </c>
-      <c r="M11" s="14">
-        <f t="shared" si="2"/>
+      <c r="M17" s="10">
+        <f t="shared" si="4"/>
         <v>0.96819470000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C18" s="9">
         <v>0.97027799999999997</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D18" s="9">
         <v>0.94651700000000005</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E18" s="9">
         <v>0.95686599999999999</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F18" s="9">
         <v>0.97487699999999999</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G18" s="9">
         <v>0.93933100000000003</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H18" s="9">
         <v>0.96973799999999999</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I18" s="9">
         <v>0.96315200000000001</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J18" s="9">
         <v>0.98167800000000005</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K18" s="9">
         <v>0.98814800000000003</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L18" s="9">
         <v>0.969557</v>
       </c>
-      <c r="M12" s="14">
-        <f t="shared" si="2"/>
+      <c r="M18" s="10">
+        <f t="shared" si="4"/>
         <v>0.96601420000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16" t="s">
+    <row r="19" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="16">
-        <f>AVERAGE(C10:C12)</f>
+      <c r="C19" s="11">
+        <f>AVERAGE(C16:C18)</f>
         <v>0.97913033333333332</v>
       </c>
-      <c r="D13" s="16">
-        <f t="shared" ref="D13:L13" si="4">AVERAGE(D10:D12)</f>
+      <c r="D19" s="11">
+        <f t="shared" ref="D19:L19" si="6">AVERAGE(D16:D18)</f>
         <v>0.96723000000000015</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E19" s="11">
+        <f t="shared" si="6"/>
+        <v>0.96087166666666679</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="6"/>
+        <v>0.94941466666666674</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="6"/>
+        <v>0.93945699999999999</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="6"/>
+        <v>0.96302466666666664</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="6"/>
+        <v>0.88934400000000002</v>
+      </c>
+      <c r="J19" s="11">
+        <f t="shared" si="6"/>
+        <v>0.96895699999999996</v>
+      </c>
+      <c r="K19" s="11">
+        <f t="shared" si="6"/>
+        <v>0.98710100000000001</v>
+      </c>
+      <c r="L19" s="11">
+        <f t="shared" si="6"/>
+        <v>0.96055400000000002</v>
+      </c>
+      <c r="M19" s="12">
         <f t="shared" si="4"/>
-        <v>0.96087166666666679</v>
-      </c>
-      <c r="F13" s="16">
-        <f t="shared" si="4"/>
-        <v>0.94941466666666674</v>
-      </c>
-      <c r="G13" s="16">
-        <f t="shared" si="4"/>
-        <v>0.93945699999999999</v>
-      </c>
-      <c r="H13" s="16">
-        <f t="shared" si="4"/>
-        <v>0.96302466666666664</v>
-      </c>
-      <c r="I13" s="16">
-        <f t="shared" si="4"/>
-        <v>0.88934400000000002</v>
-      </c>
-      <c r="J13" s="16">
-        <f t="shared" si="4"/>
-        <v>0.96895699999999996</v>
-      </c>
-      <c r="K13" s="16">
-        <f t="shared" si="4"/>
-        <v>0.98710100000000001</v>
-      </c>
-      <c r="L13" s="16">
-        <f t="shared" si="4"/>
-        <v>0.96055400000000002</v>
-      </c>
-      <c r="M13" s="17">
-        <f t="shared" si="2"/>
         <v>0.95650843333333335</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C23" s="7">
         <v>0.96643800000000002</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D23" s="7">
         <v>0.95671499999999998</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E23" s="7">
         <v>0.92356300000000002</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F23" s="7">
         <v>0.80973499999999998</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G23" s="7">
         <v>0.92954800000000004</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H23" s="7">
         <v>0.95445899999999995</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I23" s="7">
         <v>0.87846999999999997</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J23" s="7">
         <v>0.93027000000000004</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K23" s="7">
         <v>0.97466600000000003</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L23" s="7">
         <v>0.91800999999999999</v>
       </c>
-      <c r="M17" s="11">
-        <f t="shared" ref="M17:M32" si="5">AVERAGE(C17:L17)</f>
+      <c r="M23" s="8">
+        <f t="shared" ref="M23:M38" si="7">AVERAGE(C23:L23)</f>
         <v>0.9241874000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C24" s="9">
         <v>0.99470700000000001</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D24" s="9">
         <v>0.99196399999999996</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E24" s="9">
         <v>0.975939</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F24" s="9">
         <v>0.87174099999999999</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G24" s="9">
         <v>0.95522700000000005</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H24" s="9">
         <v>0.981375</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I24" s="9">
         <v>0.92851099999999998</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J24" s="9">
         <v>0.961816</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K24" s="9">
         <v>0.98932500000000001</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L24" s="9">
         <v>0.965422</v>
       </c>
-      <c r="M18" s="14">
-        <f t="shared" si="5"/>
+      <c r="M24" s="10">
+        <f t="shared" si="7"/>
         <v>0.96160269999999992</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C25" s="9">
         <v>0.96367499999999995</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D25" s="9">
         <v>0.951546</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E25" s="9">
         <v>0.93102200000000002</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F25" s="9">
         <v>0.963731</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G25" s="9">
         <v>0.94467000000000001</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H25" s="9">
         <v>0.96697299999999997</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I25" s="9">
         <v>0.97032700000000005</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J25" s="9">
         <v>0.97793699999999995</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K25" s="9">
         <v>0.98270000000000002</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L25" s="9">
         <v>0.95563799999999999</v>
       </c>
-      <c r="M19" s="14">
-        <f t="shared" si="5"/>
+      <c r="M25" s="10">
+        <f t="shared" si="7"/>
         <v>0.96082190000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16" t="s">
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="16">
-        <f t="shared" ref="C20:L20" si="6">AVERAGE(C17:C19)</f>
+      <c r="C26" s="11">
+        <f t="shared" ref="C26:L26" si="8">AVERAGE(C23:C25)</f>
         <v>0.97494000000000003</v>
       </c>
-      <c r="D20" s="16">
-        <f t="shared" si="6"/>
+      <c r="D26" s="11">
+        <f t="shared" si="8"/>
         <v>0.96674166666666661</v>
       </c>
-      <c r="E20" s="16">
-        <f t="shared" si="6"/>
+      <c r="E26" s="11">
+        <f t="shared" si="8"/>
         <v>0.94350800000000001</v>
       </c>
-      <c r="F20" s="16">
-        <f t="shared" si="6"/>
+      <c r="F26" s="11">
+        <f t="shared" si="8"/>
         <v>0.8817356666666667</v>
       </c>
-      <c r="G20" s="16">
-        <f t="shared" si="6"/>
+      <c r="G26" s="11">
+        <f t="shared" si="8"/>
         <v>0.94314833333333337</v>
       </c>
-      <c r="H20" s="16">
-        <f t="shared" si="6"/>
+      <c r="H26" s="11">
+        <f t="shared" si="8"/>
         <v>0.96760233333333323</v>
       </c>
-      <c r="I20" s="16">
-        <f t="shared" si="6"/>
+      <c r="I26" s="11">
+        <f t="shared" si="8"/>
         <v>0.92576933333333333</v>
       </c>
-      <c r="J20" s="16">
-        <f t="shared" si="6"/>
+      <c r="J26" s="11">
+        <f t="shared" si="8"/>
         <v>0.95667433333333329</v>
       </c>
-      <c r="K20" s="16">
-        <f t="shared" si="6"/>
+      <c r="K26" s="11">
+        <f t="shared" si="8"/>
         <v>0.98223033333333332</v>
       </c>
-      <c r="L20" s="16">
-        <f t="shared" si="6"/>
+      <c r="L26" s="11">
+        <f t="shared" si="8"/>
         <v>0.94635666666666662</v>
       </c>
-      <c r="M20" s="17">
-        <f t="shared" si="5"/>
+      <c r="M26" s="12">
+        <f t="shared" si="7"/>
         <v>0.94887066666666653</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C27" s="7">
         <v>0.96987299999999999</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D27" s="7">
         <v>0.94962400000000002</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E27" s="7">
         <v>0.94253799999999999</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F27" s="7">
         <v>0.85159600000000002</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G27" s="7">
         <v>0.92920400000000003</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H27" s="7">
         <v>0.92022999999999999</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I27" s="7">
         <v>0.87284799999999996</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J27" s="7">
         <v>0.90371000000000001</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K27" s="7">
         <v>0.96486899999999998</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L27" s="7">
         <v>0.937782</v>
       </c>
-      <c r="M21" s="11">
-        <f t="shared" si="5"/>
+      <c r="M27" s="8">
+        <f t="shared" si="7"/>
         <v>0.92422740000000014</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C28" s="9">
         <v>0.99517100000000003</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D28" s="9">
         <v>0.99026800000000004</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E28" s="9">
         <v>0.98357399999999995</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F28" s="9">
         <v>0.89833700000000005</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G28" s="9">
         <v>0.95590600000000003</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H28" s="9">
         <v>0.96412600000000004</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I28" s="9">
         <v>0.92574500000000004</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J28" s="9">
         <v>0.945079</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K28" s="9">
         <v>0.98505399999999999</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L28" s="9">
         <v>0.97422200000000003</v>
       </c>
-      <c r="M22" s="14">
-        <f t="shared" si="5"/>
+      <c r="M28" s="10">
+        <f t="shared" si="7"/>
         <v>0.96174819999999994</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C29" s="9">
         <v>0.97022299999999995</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D29" s="9">
         <v>0.95323800000000003</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E29" s="9">
         <v>0.95780799999999999</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F29" s="9">
         <v>0.95069599999999999</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G29" s="9">
         <v>0.95005499999999998</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H29" s="9">
         <v>0.91956099999999996</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I29" s="9">
         <v>0.969171</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J29" s="9">
         <v>0.97500900000000001</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K29" s="9">
         <v>0.98112699999999997</v>
       </c>
-      <c r="L23" s="13">
+      <c r="L29" s="9">
         <v>0.95071000000000006</v>
       </c>
-      <c r="M23" s="14">
-        <f t="shared" si="5"/>
+      <c r="M29" s="10">
+        <f t="shared" si="7"/>
         <v>0.95775980000000016</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16" t="s">
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
+      <c r="B30" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="16">
-        <f>AVERAGE(C21:C23)</f>
+      <c r="C30" s="11">
+        <f>AVERAGE(C27:C29)</f>
         <v>0.97842233333333339</v>
       </c>
-      <c r="D24" s="16">
-        <f t="shared" ref="D24:L24" si="7">AVERAGE(D21:D23)</f>
+      <c r="D30" s="11">
+        <f t="shared" ref="D30:L30" si="9">AVERAGE(D27:D29)</f>
         <v>0.96437666666666677</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E30" s="11">
+        <f t="shared" si="9"/>
+        <v>0.96130666666666664</v>
+      </c>
+      <c r="F30" s="11">
+        <f t="shared" si="9"/>
+        <v>0.90020966666666669</v>
+      </c>
+      <c r="G30" s="11">
+        <f t="shared" si="9"/>
+        <v>0.94505499999999998</v>
+      </c>
+      <c r="H30" s="11">
+        <f t="shared" si="9"/>
+        <v>0.93463899999999989</v>
+      </c>
+      <c r="I30" s="11">
+        <f t="shared" si="9"/>
+        <v>0.92258799999999985</v>
+      </c>
+      <c r="J30" s="11">
+        <f t="shared" si="9"/>
+        <v>0.94126600000000005</v>
+      </c>
+      <c r="K30" s="11">
+        <f t="shared" si="9"/>
+        <v>0.97701666666666664</v>
+      </c>
+      <c r="L30" s="11">
+        <f t="shared" si="9"/>
+        <v>0.95423800000000003</v>
+      </c>
+      <c r="M30" s="12">
         <f t="shared" si="7"/>
+        <v>0.94791179999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.972298</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0.96359399999999995</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0.94253799999999999</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.92036200000000001</v>
+      </c>
+      <c r="G31" s="7">
+        <v>0.93658200000000003</v>
+      </c>
+      <c r="H31" s="7">
+        <v>0.94107200000000002</v>
+      </c>
+      <c r="I31" s="7">
+        <v>0.83718499999999996</v>
+      </c>
+      <c r="J31" s="7">
+        <v>0.95057199999999997</v>
+      </c>
+      <c r="K31" s="7">
+        <v>0.97831900000000005</v>
+      </c>
+      <c r="L31" s="7">
+        <v>0.93449899999999997</v>
+      </c>
+      <c r="M31" s="8">
+        <f t="shared" si="7"/>
+        <v>0.93770210000000009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.99589399999999995</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.99316499999999996</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0.98357399999999995</v>
+      </c>
+      <c r="F32" s="9">
+        <v>0.94635000000000002</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0.95994500000000005</v>
+      </c>
+      <c r="H32" s="9">
+        <v>0.97604500000000005</v>
+      </c>
+      <c r="I32" s="9">
+        <v>0.90846099999999996</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.97286399999999995</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0.99122200000000005</v>
+      </c>
+      <c r="L32" s="9">
+        <v>0.973325</v>
+      </c>
+      <c r="M32" s="10">
+        <f t="shared" si="7"/>
+        <v>0.97008450000000013</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0.971271</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.94777900000000004</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0.95780799999999999</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0.972665</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0.94849799999999995</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0.96867300000000001</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0.95501000000000003</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.98150099999999996</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0.98614999999999997</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0.96833400000000003</v>
+      </c>
+      <c r="M33" s="10">
+        <f t="shared" si="7"/>
+        <v>0.96576889999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="11">
+        <f>AVERAGE(C31:C33)</f>
+        <v>0.97982099999999994</v>
+      </c>
+      <c r="D34" s="11">
+        <f t="shared" ref="D34:L34" si="10">AVERAGE(D31:D33)</f>
+        <v>0.96817933333333339</v>
+      </c>
+      <c r="E34" s="11">
+        <f t="shared" si="10"/>
         <v>0.96130666666666664</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F34" s="11">
+        <f t="shared" si="10"/>
+        <v>0.94645900000000005</v>
+      </c>
+      <c r="G34" s="11">
+        <f t="shared" si="10"/>
+        <v>0.94834166666666675</v>
+      </c>
+      <c r="H34" s="11">
+        <f t="shared" si="10"/>
+        <v>0.96193000000000006</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" si="10"/>
+        <v>0.90021866666666661</v>
+      </c>
+      <c r="J34" s="11">
+        <f t="shared" si="10"/>
+        <v>0.96831233333333333</v>
+      </c>
+      <c r="K34" s="11">
+        <f t="shared" si="10"/>
+        <v>0.98523033333333332</v>
+      </c>
+      <c r="L34" s="11">
+        <f t="shared" si="10"/>
+        <v>0.95871933333333337</v>
+      </c>
+      <c r="M34" s="12">
         <f t="shared" si="7"/>
-        <v>0.90020966666666669</v>
-      </c>
-      <c r="G24" s="16">
+        <v>0.95785183333333335</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.98099499999999995</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.95910499999999999</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.96956200000000003</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.91830900000000004</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0.96897200000000006</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.95016100000000003</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0.94304699999999997</v>
+      </c>
+      <c r="J35" s="7">
+        <v>0.91418100000000002</v>
+      </c>
+      <c r="K35" s="7">
+        <v>0.94465500000000002</v>
+      </c>
+      <c r="L35" s="7">
+        <v>0.94816500000000004</v>
+      </c>
+      <c r="M35" s="8">
         <f t="shared" si="7"/>
-        <v>0.94505499999999998</v>
-      </c>
-      <c r="H24" s="16">
+        <v>0.94971519999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0.98789400000000005</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0.97078399999999998</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0.98003300000000004</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0.92637599999999998</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0.97494999999999998</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0.96189199999999997</v>
+      </c>
+      <c r="I36" s="9">
+        <v>0.96956100000000001</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.94662000000000002</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0.94567000000000001</v>
+      </c>
+      <c r="L36" s="9">
+        <v>0.96424500000000002</v>
+      </c>
+      <c r="M36" s="10">
         <f t="shared" si="7"/>
-        <v>0.93463899999999989</v>
-      </c>
-      <c r="I24" s="16">
+        <v>0.96280249999999989</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0.97766699999999995</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0.88446800000000003</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0.97835000000000005</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0.98145199999999999</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0.77866299999999999</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0.94178600000000001</v>
+      </c>
+      <c r="I37" s="9">
+        <v>0.92081000000000002</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0.86926899999999996</v>
+      </c>
+      <c r="K37" s="9">
+        <v>0.88734599999999997</v>
+      </c>
+      <c r="L37" s="9">
+        <v>0.97290399999999999</v>
+      </c>
+      <c r="M37" s="10">
         <f t="shared" si="7"/>
-        <v>0.92258799999999985</v>
-      </c>
-      <c r="J24" s="16">
+        <v>0.91927150000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
+      <c r="B38" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="11">
+        <f>AVERAGE(C35:C37)</f>
+        <v>0.98218533333333324</v>
+      </c>
+      <c r="D38" s="11">
+        <f t="shared" ref="D38" si="11">AVERAGE(D35:D37)</f>
+        <v>0.93811900000000004</v>
+      </c>
+      <c r="E38" s="11">
+        <f t="shared" ref="E38" si="12">AVERAGE(E35:E37)</f>
+        <v>0.97598166666666675</v>
+      </c>
+      <c r="F38" s="11">
+        <f t="shared" ref="F38" si="13">AVERAGE(F35:F37)</f>
+        <v>0.94204566666666667</v>
+      </c>
+      <c r="G38" s="11">
+        <f t="shared" ref="G38" si="14">AVERAGE(G35:G37)</f>
+        <v>0.90752833333333338</v>
+      </c>
+      <c r="H38" s="11">
+        <f t="shared" ref="H38" si="15">AVERAGE(H35:H37)</f>
+        <v>0.95127966666666663</v>
+      </c>
+      <c r="I38" s="11">
+        <f t="shared" ref="I38" si="16">AVERAGE(I35:I37)</f>
+        <v>0.94447266666666663</v>
+      </c>
+      <c r="J38" s="11">
+        <f t="shared" ref="J38" si="17">AVERAGE(J35:J37)</f>
+        <v>0.9100233333333333</v>
+      </c>
+      <c r="K38" s="11">
+        <f t="shared" ref="K38" si="18">AVERAGE(K35:K37)</f>
+        <v>0.92589033333333326</v>
+      </c>
+      <c r="L38" s="11">
+        <f t="shared" ref="L38" si="19">AVERAGE(L35:L37)</f>
+        <v>0.96177133333333342</v>
+      </c>
+      <c r="M38" s="12">
         <f t="shared" si="7"/>
-        <v>0.94126600000000005</v>
-      </c>
-      <c r="K24" s="16">
-        <f t="shared" si="7"/>
-        <v>0.97701666666666664</v>
-      </c>
-      <c r="L24" s="16">
-        <f t="shared" si="7"/>
-        <v>0.95423800000000003</v>
-      </c>
-      <c r="M24" s="17">
-        <f t="shared" si="5"/>
-        <v>0.94791179999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="10" t="s">
+        <v>0.94392973333333319</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="10">
-        <v>0.972298</v>
-      </c>
-      <c r="D25" s="10">
-        <v>0.96359399999999995</v>
-      </c>
-      <c r="E25" s="10">
-        <v>0.94253799999999999</v>
-      </c>
-      <c r="F25" s="10">
-        <v>0.92036200000000001</v>
-      </c>
-      <c r="G25" s="10">
-        <v>0.93658200000000003</v>
-      </c>
-      <c r="H25" s="10">
-        <v>0.94107200000000002</v>
-      </c>
-      <c r="I25" s="10">
-        <v>0.83718499999999996</v>
-      </c>
-      <c r="J25" s="10">
-        <v>0.95057199999999997</v>
-      </c>
-      <c r="K25" s="10">
-        <v>0.97831900000000005</v>
-      </c>
-      <c r="L25" s="10">
-        <v>0.93449899999999997</v>
-      </c>
-      <c r="M25" s="11">
-        <f t="shared" si="5"/>
-        <v>0.93770210000000009</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13" t="s">
+      <c r="C40" s="7">
+        <v>0.985707</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0.97549200000000003</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.97760599999999998</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.94688000000000005</v>
+      </c>
+      <c r="G40" s="7">
+        <v>0.98402900000000004</v>
+      </c>
+      <c r="H40" s="7">
+        <v>0.97397900000000004</v>
+      </c>
+      <c r="I40" s="7">
+        <v>0.95601199999999997</v>
+      </c>
+      <c r="J40" s="7">
+        <v>0.94150299999999998</v>
+      </c>
+      <c r="K40" s="7">
+        <v>0.98221099999999995</v>
+      </c>
+      <c r="L40" s="7">
+        <v>0.95685699999999996</v>
+      </c>
+      <c r="M40" s="8">
+        <f t="shared" ref="M40:M43" si="20">AVERAGE(C40:L40)</f>
+        <v>0.96802759999999988</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="13">
-        <v>0.99589399999999995</v>
-      </c>
-      <c r="D26" s="13">
-        <v>0.99316499999999996</v>
-      </c>
-      <c r="E26" s="13">
-        <v>0.98357399999999995</v>
-      </c>
-      <c r="F26" s="13">
-        <v>0.94635000000000002</v>
-      </c>
-      <c r="G26" s="13">
-        <v>0.95994500000000005</v>
-      </c>
-      <c r="H26" s="13">
-        <v>0.97604500000000005</v>
-      </c>
-      <c r="I26" s="13">
-        <v>0.90846099999999996</v>
-      </c>
-      <c r="J26" s="13">
-        <v>0.97286399999999995</v>
-      </c>
-      <c r="K26" s="13">
-        <v>0.99122200000000005</v>
-      </c>
-      <c r="L26" s="13">
-        <v>0.973325</v>
-      </c>
-      <c r="M26" s="14">
-        <f t="shared" si="5"/>
-        <v>0.97008450000000013</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13" t="s">
+      <c r="C41" s="9">
+        <v>0.99811099999999997</v>
+      </c>
+      <c r="D41" s="9">
+        <v>0.99560000000000004</v>
+      </c>
+      <c r="E41" s="9">
+        <v>0.99313799999999997</v>
+      </c>
+      <c r="F41" s="9">
+        <v>0.965279</v>
+      </c>
+      <c r="G41" s="9">
+        <v>0.99390900000000004</v>
+      </c>
+      <c r="H41" s="9">
+        <v>0.98983500000000002</v>
+      </c>
+      <c r="I41" s="9">
+        <v>0.981159</v>
+      </c>
+      <c r="J41" s="9">
+        <v>0.96987599999999996</v>
+      </c>
+      <c r="K41" s="9">
+        <v>0.99289300000000003</v>
+      </c>
+      <c r="L41" s="9">
+        <v>0.980236</v>
+      </c>
+      <c r="M41" s="10">
+        <f t="shared" si="20"/>
+        <v>0.98600360000000009</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="13">
-        <v>0.971271</v>
-      </c>
-      <c r="D27" s="13">
-        <v>0.94777900000000004</v>
-      </c>
-      <c r="E27" s="13">
-        <v>0.95780799999999999</v>
-      </c>
-      <c r="F27" s="13">
-        <v>0.972665</v>
-      </c>
-      <c r="G27" s="13">
-        <v>0.94849799999999995</v>
-      </c>
-      <c r="H27" s="13">
-        <v>0.96867300000000001</v>
-      </c>
-      <c r="I27" s="13">
-        <v>0.95501000000000003</v>
-      </c>
-      <c r="J27" s="13">
-        <v>0.98150099999999996</v>
-      </c>
-      <c r="K27" s="13">
-        <v>0.98614999999999997</v>
-      </c>
-      <c r="L27" s="13">
-        <v>0.96833400000000003</v>
-      </c>
-      <c r="M27" s="14">
-        <f t="shared" si="5"/>
-        <v>0.96576889999999993</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16" t="s">
+      <c r="C42" s="9">
+        <v>0.98219100000000004</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0.943573</v>
+      </c>
+      <c r="E42" s="9">
+        <v>0.98261900000000002</v>
+      </c>
+      <c r="F42" s="9">
+        <v>0.98596799999999996</v>
+      </c>
+      <c r="G42" s="9">
+        <v>0.86264300000000005</v>
+      </c>
+      <c r="H42" s="9">
+        <v>0.98279399999999995</v>
+      </c>
+      <c r="I42" s="9">
+        <v>0.98171399999999998</v>
+      </c>
+      <c r="J42" s="9">
+        <v>0.980159</v>
+      </c>
+      <c r="K42" s="9">
+        <v>0.98742300000000005</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0.97774700000000003</v>
+      </c>
+      <c r="M42" s="10">
+        <f t="shared" si="20"/>
+        <v>0.96668310000000024</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="16"/>
+      <c r="B43" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="16">
-        <f>AVERAGE(C25:C27)</f>
-        <v>0.97982099999999994</v>
-      </c>
-      <c r="D28" s="16">
-        <f t="shared" ref="D28:L28" si="8">AVERAGE(D25:D27)</f>
-        <v>0.96817933333333339</v>
-      </c>
-      <c r="E28" s="16">
-        <f t="shared" si="8"/>
-        <v>0.96130666666666664</v>
-      </c>
-      <c r="F28" s="16">
-        <f t="shared" si="8"/>
-        <v>0.94645900000000005</v>
-      </c>
-      <c r="G28" s="16">
-        <f t="shared" si="8"/>
-        <v>0.94834166666666675</v>
-      </c>
-      <c r="H28" s="16">
-        <f t="shared" si="8"/>
-        <v>0.96193000000000006</v>
-      </c>
-      <c r="I28" s="16">
-        <f t="shared" si="8"/>
-        <v>0.90021866666666661</v>
-      </c>
-      <c r="J28" s="16">
-        <f t="shared" si="8"/>
-        <v>0.96831233333333333</v>
-      </c>
-      <c r="K28" s="16">
-        <f t="shared" si="8"/>
-        <v>0.98523033333333332</v>
-      </c>
-      <c r="L28" s="16">
-        <f t="shared" si="8"/>
-        <v>0.95871933333333337</v>
-      </c>
-      <c r="M28" s="17">
-        <f t="shared" si="5"/>
-        <v>0.95785183333333335</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="10">
-        <v>0.98099499999999995</v>
-      </c>
-      <c r="D29" s="10">
-        <v>0.95910499999999999</v>
-      </c>
-      <c r="E29" s="10">
-        <v>0.96956200000000003</v>
-      </c>
-      <c r="F29" s="10">
-        <v>0.91830900000000004</v>
-      </c>
-      <c r="G29" s="10">
-        <v>0.96897200000000006</v>
-      </c>
-      <c r="H29" s="10">
-        <v>0.95016100000000003</v>
-      </c>
-      <c r="I29" s="10">
-        <v>0.94304699999999997</v>
-      </c>
-      <c r="J29" s="10">
-        <v>0.91418100000000002</v>
-      </c>
-      <c r="K29" s="10">
-        <v>0.94465500000000002</v>
-      </c>
-      <c r="L29" s="10">
-        <v>0.94816500000000004</v>
-      </c>
-      <c r="M29" s="11">
-        <f t="shared" si="5"/>
-        <v>0.94971519999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="13">
-        <v>0.98789400000000005</v>
-      </c>
-      <c r="D30" s="13">
-        <v>0.97078399999999998</v>
-      </c>
-      <c r="E30" s="13">
-        <v>0.98003300000000004</v>
-      </c>
-      <c r="F30" s="13">
-        <v>0.92637599999999998</v>
-      </c>
-      <c r="G30" s="13">
-        <v>0.97494999999999998</v>
-      </c>
-      <c r="H30" s="13">
-        <v>0.96189199999999997</v>
-      </c>
-      <c r="I30" s="13">
-        <v>0.96956100000000001</v>
-      </c>
-      <c r="J30" s="13">
-        <v>0.94662000000000002</v>
-      </c>
-      <c r="K30" s="13">
-        <v>0.94567000000000001</v>
-      </c>
-      <c r="L30" s="13">
-        <v>0.96424500000000002</v>
-      </c>
-      <c r="M30" s="14">
-        <f t="shared" si="5"/>
-        <v>0.96280249999999989</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="13">
-        <v>0.97766699999999995</v>
-      </c>
-      <c r="D31" s="13">
-        <v>0.88446800000000003</v>
-      </c>
-      <c r="E31" s="13">
-        <v>0.97835000000000005</v>
-      </c>
-      <c r="F31" s="13">
-        <v>0.98145199999999999</v>
-      </c>
-      <c r="G31" s="13">
-        <v>0.77866299999999999</v>
-      </c>
-      <c r="H31" s="13">
-        <v>0.94178600000000001</v>
-      </c>
-      <c r="I31" s="13">
-        <v>0.92081000000000002</v>
-      </c>
-      <c r="J31" s="13">
-        <v>0.86926899999999996</v>
-      </c>
-      <c r="K31" s="13">
-        <v>0.88734599999999997</v>
-      </c>
-      <c r="L31" s="13">
-        <v>0.97290399999999999</v>
-      </c>
-      <c r="M31" s="14">
-        <f t="shared" si="5"/>
-        <v>0.91927150000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="16">
-        <f>AVERAGE(C29:C31)</f>
-        <v>0.98218533333333324</v>
-      </c>
-      <c r="D32" s="16">
-        <f t="shared" ref="D32" si="9">AVERAGE(D29:D31)</f>
-        <v>0.93811900000000004</v>
-      </c>
-      <c r="E32" s="16">
-        <f t="shared" ref="E32" si="10">AVERAGE(E29:E31)</f>
-        <v>0.97598166666666675</v>
-      </c>
-      <c r="F32" s="16">
-        <f t="shared" ref="F32" si="11">AVERAGE(F29:F31)</f>
-        <v>0.94204566666666667</v>
-      </c>
-      <c r="G32" s="16">
-        <f t="shared" ref="G32" si="12">AVERAGE(G29:G31)</f>
-        <v>0.90752833333333338</v>
-      </c>
-      <c r="H32" s="16">
-        <f t="shared" ref="H32" si="13">AVERAGE(H29:H31)</f>
-        <v>0.95127966666666663</v>
-      </c>
-      <c r="I32" s="16">
-        <f t="shared" ref="I32" si="14">AVERAGE(I29:I31)</f>
-        <v>0.94447266666666663</v>
-      </c>
-      <c r="J32" s="16">
-        <f t="shared" ref="J32" si="15">AVERAGE(J29:J31)</f>
-        <v>0.9100233333333333</v>
-      </c>
-      <c r="K32" s="16">
-        <f t="shared" ref="K32" si="16">AVERAGE(K29:K31)</f>
-        <v>0.92589033333333326</v>
-      </c>
-      <c r="L32" s="16">
-        <f t="shared" ref="L32" si="17">AVERAGE(L29:L31)</f>
-        <v>0.96177133333333342</v>
-      </c>
-      <c r="M32" s="17">
-        <f t="shared" si="5"/>
-        <v>0.94392973333333319</v>
+      <c r="C43" s="11">
+        <f>AVERAGE(C40:C42)</f>
+        <v>0.98866966666666656</v>
+      </c>
+      <c r="D43" s="11">
+        <f t="shared" ref="D43:L43" si="21">AVERAGE(D40:D42)</f>
+        <v>0.97155500000000006</v>
+      </c>
+      <c r="E43" s="11">
+        <f t="shared" si="21"/>
+        <v>0.98445433333333332</v>
+      </c>
+      <c r="F43" s="11">
+        <f t="shared" si="21"/>
+        <v>0.96604233333333323</v>
+      </c>
+      <c r="G43" s="11">
+        <f t="shared" si="21"/>
+        <v>0.94686033333333341</v>
+      </c>
+      <c r="H43" s="11">
+        <f t="shared" si="21"/>
+        <v>0.98220266666666678</v>
+      </c>
+      <c r="I43" s="11">
+        <f t="shared" si="21"/>
+        <v>0.97296166666666661</v>
+      </c>
+      <c r="J43" s="11">
+        <f t="shared" si="21"/>
+        <v>0.96384599999999987</v>
+      </c>
+      <c r="K43" s="11">
+        <f t="shared" si="21"/>
+        <v>0.98750900000000008</v>
+      </c>
+      <c r="L43" s="11">
+        <f t="shared" si="21"/>
+        <v>0.97161333333333333</v>
+      </c>
+      <c r="M43" s="12">
+        <f t="shared" si="20"/>
+        <v>0.9735714333333334</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A25:A28"/>
+  <mergeCells count="10">
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A27:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1904,7 +2259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -1915,24 +2270,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1968,7 +2323,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2010,7 +2365,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2050,7 +2405,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2090,7 +2445,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2140,7 +2495,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2182,7 +2537,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2222,7 +2577,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2262,7 +2617,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -2312,7 +2667,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2354,7 +2709,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2394,7 +2749,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -2434,7 +2789,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
@@ -2484,7 +2839,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2526,7 +2881,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -2566,7 +2921,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -2606,7 +2961,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
@@ -2656,7 +3011,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2698,7 +3053,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
@@ -2738,7 +3093,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2778,7 +3133,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
@@ -2831,26 +3186,26 @@
       <c r="A23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
     </row>
     <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="4" t="s">
         <v>13</v>
       </c>
@@ -2886,7 +3241,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2928,7 +3283,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
@@ -2968,7 +3323,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
@@ -3008,7 +3363,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="3" t="s">
         <v>6</v>
       </c>
@@ -3058,7 +3413,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -3100,7 +3455,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
@@ -3140,7 +3495,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
@@ -3180,7 +3535,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
@@ -3230,7 +3585,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -3272,7 +3627,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
@@ -3312,7 +3667,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3352,7 +3707,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
@@ -3402,7 +3757,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3444,7 +3799,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
@@ -3484,7 +3839,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
@@ -3524,7 +3879,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="3" t="s">
         <v>6</v>
       </c>
@@ -3574,7 +3929,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -3616,7 +3971,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="1" t="s">
         <v>4</v>
       </c>
@@ -3656,7 +4011,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
@@ -3696,7 +4051,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
@@ -3781,24 +4136,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3834,7 +4189,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3876,7 +4231,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3916,7 +4271,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -3956,7 +4311,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -4006,7 +4361,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -4048,7 +4403,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -4088,7 +4443,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -4128,7 +4483,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -4178,7 +4533,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -4220,7 +4575,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
@@ -4260,7 +4615,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -4300,7 +4655,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
@@ -4350,7 +4705,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -4392,7 +4747,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -4432,7 +4787,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -4472,7 +4827,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
@@ -4522,7 +4877,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -4564,7 +4919,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
@@ -4604,7 +4959,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
@@ -4644,7 +4999,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
@@ -4697,26 +5052,26 @@
       <c r="A23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
     </row>
     <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="4" t="s">
         <v>13</v>
       </c>
@@ -4752,7 +5107,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -4794,7 +5149,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
@@ -4834,7 +5189,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
@@ -4874,7 +5229,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="3" t="s">
         <v>6</v>
       </c>
@@ -4924,7 +5279,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -4966,7 +5321,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
@@ -5006,7 +5361,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
@@ -5046,7 +5401,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
@@ -5096,7 +5451,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -5138,7 +5493,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
@@ -5178,7 +5533,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
@@ -5218,7 +5573,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
@@ -5268,7 +5623,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -5310,7 +5665,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
@@ -5350,7 +5705,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
@@ -5390,7 +5745,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="3" t="s">
         <v>6</v>
       </c>
@@ -5440,7 +5795,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -5482,7 +5837,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="1" t="s">
         <v>4</v>
       </c>
@@ -5522,7 +5877,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
@@ -5562,7 +5917,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
@@ -5613,12 +5968,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A19:A22"/>
@@ -5627,6 +5976,12 @@
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>